<commit_message>
Update excel file with extracted nouns
</commit_message>
<xml_diff>
--- a/hg.xlsx
+++ b/hg.xlsx
@@ -450,77 +450,77 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>일단 ai의 수준차이도 나면서 빈부격차가 더 심해질거 같다</t>
+          <t>일단 수준 차이 빈부격차</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ai가 직업들을 없애버릴 수 있는 상황이 벌어질 수 있다.</t>
+          <t>직업 상황</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ai가 오작동해 사람의 생명을 위협할 수 있는 상황도 나온다.</t>
+          <t>동해 사람 생명 위협 상황</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>자율주행 AI가 교통사고를 냈을 때 책임을 묻기가 힘들다.</t>
+          <t>자율 주행 교통사고 책임</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>일자리에 위협이 될수 있다.</t>
+          <t>일자리 위협</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>무분별한 데이터 수집으로 인한 저작권 침해</t>
+          <t>무분별 데이터 수집 저작권 침해</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>잘못된 데이터 수집으로 인한 가짜 뉴스 확산</t>
+          <t>데이터 수집 가짜 뉴스 확산</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ai 활용 사이버 테러 증가</t>
+          <t>활용 사이버 테러 증가</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ai 딥페이크와 목소리 모방 기술로 인한 피해</t>
+          <t>페이크 목소리 모방 기술 피해</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ai가 질문을 통해 쉽게 답을 해줘서 일자리 감소를 발생시킨다.</t>
+          <t>질문 통해 일자리 감소 발생</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>세계지배.</t>
+          <t>세계 지배</t>
         </is>
       </c>
     </row>
@@ -530,616 +530,612 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ai가 사람의 일자리를 감소시킨다.</t>
+          <t>사람 일자리 감소</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>빠르게 발전하면 제어를 하기 힘들다.</t>
+          <t>발전 제어</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>범죄에 악용 당할 수 있다.</t>
+          <t>범죄 악용</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>전쟁 범죄에 쓰일 수 있다.</t>
+          <t>전쟁 범죄</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>전쟁에 악용될 수 있다.</t>
+          <t>전쟁 악용</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>개인정보가 털릴 수 있다.</t>
+          <t>개인정보</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ai의 수준차이도 나면서 빈부격차가 더 심해질거 같으며 ai가 모든 직업에 나서게 된다면 사람들의 가난이 더 지속될 것이다.</t>
+          <t>수준 차이 빈부격차 모든 직업 사람 가난 지속</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>딥페이크를 통해 사칭 위험성이 있다.</t>
+          <t>페이크 통해 사칭 위험성</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>사람들이 ai를 악용과 남용을 할 수 있다.</t>
+          <t>사람 악용 남용</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>사람들의 사고 능력을 하락 시킨다.</t>
+          <t>사람 사고 능력 하락</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">인공지능은 매우 위험하다고 생각하지 않습니다. </t>
+          <t>인공 지능 매우 생각</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">안전하게 활용되기 위해서는 인공지능은 우리 삶에서 배제 되서는 안됩니다. </t>
+          <t>활용 인공 지능 우리 배제</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">딥페이크 이미지를 악용하는데 불법적으로 활용된다. </t>
+          <t>페이크 이미지 악용 불법 활용</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AI 딥페이크 기술 및 더빙 기술이 악용되어 살아있는 사람 뿐만 아니라 돌아가신 고인에게도 명예훼손을 입힐 가능성이 있음.</t>
+          <t>페이크 기술 더빙 기술 악용 사람 고인 명예훼손 가능성</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>많은 일자리 감소 , ai를 이용한 얼굴 합성 (딥페이크)</t>
+          <t>일자리 감소 이용 얼굴 합성 페이크</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ai가 발달하다보면 차후에 사람들의 일자리를 다 빼앗을 가능성이 있기에 위험하다.</t>
+          <t>발달 차후 사람 일자리 가능성</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ai가 점점 사람과 비슷해지면서 만약 자아를 이뤘는데 통제가 안될 수도 있고 그에 따른 위험이 있을 것이다.</t>
+          <t>점점 사람과 만약 자아 통제 수도 위험</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>급격한 발전으로 인해 인간의 일자리 등을 많이 빼앗고 있다</t>
+          <t>발전 인간 일자리</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>매우 위헌해요</t>
+          <t>매우</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ai가 더욱더 발전한다면 정말 미래에 실업률이 급격하게 증가할 것이다. </t>
+          <t>더욱더 발전 정말 미래 실업률 증가</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>미래에 인공지능은 뛰어난 학습 능력과 환경 적응 능력, 그리고 인간보다 대부분의 면에서 월들히 뛰어난 모습을 보여주어 전 세계의 적업의 60%가 사라지게 되어 인간들이 직업을 찾기가 더욱 힘들어진다는 위험성이 있다.</t>
+          <t>미래 인공 지능 학습 능력 환경 적응 능력 인간 대부분 모습 세계 적업 인간 직업 찾기 더욱 위험성</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>우리가 성인이 됐을때 ai가 우리의 직업을 뺏어서 우리는 일을 잃게 될 것이다</t>
+          <t>우리 성인 우리 직업 우리</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ai에 빠른 발전이 우리 인간의 일자리를 점점 사라지게 만드는것이 위험성이것같다.</t>
+          <t>발전 우리 인간 일자리 점점 위험성</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ai가 대량학살이 가능하게 개조되는 순간부터 사람들끼리 서로 목숨줄을 잡고있는 상황이 될거다.</t>
+          <t>대량학살 개조 순간 사람 끼리 서로 목숨 상황</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>정말 나중에 AI가 다 해먹을지도 모를정도로 현재 AI기술이 빠르게 성장하고 있다고 생각하는데요.계속 이렇게 가다가는 정말로 수 많은 직업들이 시리질거 같아서 조금은 위험하지 않나 라고 생각합니다.</t>
+          <t>정말 나중 해먹 지도 정도 현재 기술 생각 계속 가다가 직업 시리 조금 생각</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>이제 곧 영화에서처럼 ai가 세상을 장악할 수도 있다는 생각이 들었다.</t>
+          <t>이제 영화에서처럼 세상 장악 수도 생각</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ai는 아무리 발전해도 인간은 결국 공존할 방법을 찾아낼 것이다.</t>
+          <t>발전 인간 공존 방법</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ai가 직접 사람들에게 해를 끼치는 것은 아니지만 사람들이 점점. 자신의 생각이 아닌 ai에게 맡기는 것이 위험하다</t>
+          <t>직접 사람 사람 점점 자신 생각</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>굉장히 위험하다</t>
-        </is>
-      </c>
+      <c r="A43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ai가 생활화됐을 때 일자리를 잃는 사람들이 있다</t>
+          <t>생활화 일자리 사람</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>일자리를 빼앗아간다</t>
+          <t>일자리 간다</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>사람이 멍청해짐</t>
+          <t>사람</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>일자리를 위협한다.</t>
+          <t>일자리 위협</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ai가 나중에 우리의 일자리를 다 차지 할까봐 위험한거 같음</t>
+          <t>나중 우리 일자리 차지</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AI의 기술이 점점 발달하면서 많은 사람들이 직업을 잃을수 있음.</t>
+          <t>기술 점점 발달 사람 직업</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AI로 인해 사람들의 직업들이 뺏기고 있고 사람들의 취업률 또한 줄어들고 있어 AI가 위험할지도 모른다.</t>
+          <t>사람 직업 사람 취업률 또한</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Ai가 사람보다 지능이 높아지면 앞으로 ai가 나쁘게 돌변할수도 있다</t>
+          <t>사람 지능 돌변</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>요즘 딥페이크 때문에 많은 유명인들이 피해릉 받고 있는데, 저게 더 심해지면 사기를 당할 위험이 높아질 것 같습니다</t>
+          <t>요즘 페이크 때문 유명인 피해 사기 위험</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>인간이 지배 당할 것이다.</t>
+          <t>인간 지배</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>사람의 삶이 위험해 질 것이다.</t>
+          <t>사람</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ai는 우리 삶에 유용하지만 대비를 해야 한다.</t>
+          <t>우리 대비</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>chat gpt가 발전해서 우리 삶을 위협한다.</t>
+          <t>발전 우리 위협</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>예술부터 차근차근 공격 받을 것이다.</t>
+          <t>예술 차근차근 공격</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>딥페이크 피해</t>
+          <t>페이크 피해</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ai가 인간을 지배한다.</t>
+          <t>인간 지배</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ai로 인한 일자리 감소가 많아서 위험하다.</t>
+          <t>일자리 감소</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>사이버 피해가 많아진다.</t>
+          <t>사이버 피해</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>인간이 지배당한다.</t>
+          <t>인간 지배</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>우리 삶이 피폐해진다.</t>
+          <t>우리 폐해</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>AI를 잘못 활용할경우 상상하지 못할 범죄가 일어날 수도 있고 사람들에 직업을 뺏어 사람들이 점점 할일이 없어질 것이다</t>
+          <t>잘못 활용 경우 상상 범죄 수도 사람 직업 사람 점점 일이</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>뉴스에서처럼 많은 피해자가 나올 것이다.</t>
+          <t>뉴스 피해자</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ai에 대한 법을 개정해야 한다.</t>
+          <t>대한 개정</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ai가 발전하여 사람을 공격할 수 있다.</t>
+          <t>발전 사람 공격</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ai가 인간을 조종한다.</t>
+          <t>인간 조종</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ai가 사람에 비해 똑똑해서 큰 위험이 생긴다.</t>
+          <t>사람 위험</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>실업률이 증가 할 것이다.</t>
+          <t>실업률 증가</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>인간에 대한 공격이 생길 수 있다.</t>
+          <t>인간 대한 공격</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ai가 인간의 사고를 넘어설 것이다.</t>
+          <t>인간 사고</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>사람들이 멍청해진다.</t>
+          <t>사람</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ai를 이용한 사이버 범죄가 생긴다.</t>
+          <t>이용 사이버 범죄</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ai로 인해 사람들의 지능이 낮아진다.</t>
+          <t>사람 지능</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ai가 사람을 열등하게 보면서 지배하려고 할수 있다.</t>
+          <t>사람 지배</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>사람을 공격한다.</t>
+          <t>사람 공격</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>가짜 정보가 늘어날수 있다.</t>
+          <t>가짜 정보</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ai가 대신 일을 해서 일자리가 감소한다.</t>
+          <t>대신 일자리 감소</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ai가 대신 일을 해서 일자리가 감소한다.</t>
+          <t>대신 일자리 감소</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>딥페이크 같이 신분을 악용할수 있다.</t>
+          <t>페이크 신분 악용</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>ai가 인간을 공격할수 있다.</t>
+          <t>인간 공격</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>딥페이크로 많은 사기가 생길 수 있다.</t>
+          <t>페이크 사기</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ai가 지배하려고 할수 있다.</t>
+          <t>지배</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Ai 의 위험성 8점(10점 만점)</t>
+          <t>위험성 만점</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ai가 악용될 우려가 있다.</t>
+          <t>악용 우려</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ai로 인해 잘못된 데이터가 학습될수 있다.</t>
+          <t>데이터 학습</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>윤리적 문제가 발생한다.</t>
+          <t>윤리 문제 발생</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>해킹의 위험이 있다.</t>
+          <t>해킹 위험</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ai는 도덕적이지 못한다.</t>
+          <t>도덕</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>문학의 의미가 없어진다.</t>
+          <t>문학 의미</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ai가 세상을 지배한다.</t>
+          <t>세상 지배</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ai가 자연을 파괴할수 있다.</t>
+          <t>자연 파괴</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>범죄에 악용될수 있다.</t>
+          <t>범죄 악용</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>사기가 많이 발생한다.</t>
+          <t>사기 발생</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>ai가 사람들의 범죄에 악용된다.</t>
+          <t>사람 범죄 악용</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>ai가 새로운 범죄를 만든다.</t>
+          <t>범죄</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>사이버 범죄가 많이 생긴다.</t>
+          <t>사이버 범죄</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>ai의 반란이 일어난다.</t>
+          <t>반란 일어난다</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>ai가 오류를 일으키면 막을수 없다.</t>
+          <t>오류</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ai에 대한 규제를 빠르게 만들어야 한다.</t>
+          <t>대한 규제</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>직업 사라짐</t>
+          <t>직업</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update excel file with extracted verbs
</commit_message>
<xml_diff>
--- a/hg.xlsx
+++ b/hg.xlsx
@@ -441,703 +441,307 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>발전 인간 공격 생각</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>일단 수준 차이 빈부격차</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>직업 상황</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>동해 사람 생명 위협 상황</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>자율 주행 교통사고 책임</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>일자리 위협</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>무분별 데이터 수집 저작권 침해</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>데이터 수집 가짜 뉴스 확산</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>활용 사이버 테러 증가</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>페이크 목소리 모방 기술 피해</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>질문 통해 일자리 감소 발생</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>세계 지배</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>사람 일자리 감소</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>발전 제어</t>
-        </is>
-      </c>
+      <c r="A16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>범죄 악용</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>전쟁 범죄</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>전쟁 악용</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>개인정보</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>수준 차이 빈부격차 모든 직업 사람 가난 지속</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>페이크 통해 사칭 위험성</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>사람 악용 남용</t>
-        </is>
-      </c>
+      <c r="A23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>사람 사고 능력 하락</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>인공 지능 매우 생각</t>
-        </is>
-      </c>
+      <c r="A25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>활용 인공 지능 우리 배제</t>
-        </is>
-      </c>
+      <c r="A26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>페이크 이미지 악용 불법 활용</t>
-        </is>
-      </c>
+      <c r="A27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>페이크 기술 더빙 기술 악용 사람 고인 명예훼손 가능성</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>일자리 감소 이용 얼굴 합성 페이크</t>
-        </is>
-      </c>
+      <c r="A29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>발달 차후 사람 일자리 가능성</t>
-        </is>
-      </c>
+      <c r="A30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>점점 사람과 만약 자아 통제 수도 위험</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>발전 인간 일자리</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>매우</t>
-        </is>
-      </c>
+      <c r="A33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>더욱더 발전 정말 미래 실업률 증가</t>
-        </is>
-      </c>
+      <c r="A34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>미래 인공 지능 학습 능력 환경 적응 능력 인간 대부분 모습 세계 적업 인간 직업 찾기 더욱 위험성</t>
-        </is>
-      </c>
+      <c r="A35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>우리 성인 우리 직업 우리</t>
-        </is>
-      </c>
+      <c r="A36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>발전 우리 인간 일자리 점점 위험성</t>
-        </is>
-      </c>
+      <c r="A37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>대량학살 개조 순간 사람 끼리 서로 목숨 상황</t>
-        </is>
-      </c>
+      <c r="A38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>정말 나중 해먹 지도 정도 현재 기술 생각 계속 가다가 직업 시리 조금 생각</t>
-        </is>
-      </c>
+      <c r="A39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>이제 영화에서처럼 세상 장악 수도 생각</t>
-        </is>
-      </c>
+      <c r="A40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>발전 인간 공존 방법</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>직접 사람 사람 점점 자신 생각</t>
-        </is>
-      </c>
+      <c r="A42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>생활화 일자리 사람</t>
-        </is>
-      </c>
+      <c r="A44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>일자리</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>사람</t>
-        </is>
-      </c>
+      <c r="A46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>일자리 위협</t>
-        </is>
-      </c>
+      <c r="A47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>나중 우리 일자리 차지</t>
-        </is>
-      </c>
+      <c r="A48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>기술 점점 발달 사람 직업</t>
-        </is>
-      </c>
+      <c r="A49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>사람 직업 사람 취업률 또한</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>사람 지능 돌변</t>
-        </is>
-      </c>
+      <c r="A51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>요즘 페이크 때문 유명인 피해 사기 위험</t>
-        </is>
-      </c>
+      <c r="A52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>인간 지배</t>
-        </is>
-      </c>
+      <c r="A53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>사람</t>
-        </is>
-      </c>
+      <c r="A54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>우리 대비</t>
-        </is>
-      </c>
+      <c r="A55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>발전 우리 위협</t>
-        </is>
-      </c>
+      <c r="A56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>예술 차근차근 공격</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>페이크 피해</t>
-        </is>
-      </c>
+      <c r="A58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>인간 지배</t>
-        </is>
-      </c>
+      <c r="A59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>일자리 감소</t>
-        </is>
-      </c>
+      <c r="A60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>사이버 피해</t>
-        </is>
-      </c>
+      <c r="A61" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>인간 지배</t>
-        </is>
-      </c>
+      <c r="A62" t="inlineStr"/>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>우리 폐해</t>
-        </is>
-      </c>
+      <c r="A63" t="inlineStr"/>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>잘못 활용 경우 상상 범죄 수도 사람 직업 사람 점점</t>
-        </is>
-      </c>
+      <c r="A64" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>뉴스 피해자</t>
-        </is>
-      </c>
+      <c r="A65" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>대한 개정</t>
-        </is>
-      </c>
+      <c r="A66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>발전 사람 공격</t>
-        </is>
-      </c>
+      <c r="A67" t="inlineStr"/>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>인간 조종</t>
-        </is>
-      </c>
+      <c r="A68" t="inlineStr"/>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>사람 위험</t>
-        </is>
-      </c>
+      <c r="A69" t="inlineStr"/>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>실업률 증가</t>
-        </is>
-      </c>
+      <c r="A70" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>인간 대한 공격</t>
-        </is>
-      </c>
+      <c r="A71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>인간 사고</t>
-        </is>
-      </c>
+      <c r="A72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>사람</t>
-        </is>
-      </c>
+      <c r="A73" t="inlineStr"/>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>이용 사이버 범죄</t>
-        </is>
-      </c>
+      <c r="A74" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>사람 지능</t>
-        </is>
-      </c>
+      <c r="A75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>사람 지배</t>
-        </is>
-      </c>
+      <c r="A76" t="inlineStr"/>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>사람 공격</t>
-        </is>
-      </c>
+      <c r="A77" t="inlineStr"/>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>가짜 정보</t>
-        </is>
-      </c>
+      <c r="A78" t="inlineStr"/>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>대신 일자리 감소</t>
-        </is>
-      </c>
+      <c r="A79" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>대신 일자리 감소</t>
-        </is>
-      </c>
+      <c r="A80" t="inlineStr"/>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>페이크 신분 악용</t>
-        </is>
-      </c>
+      <c r="A81" t="inlineStr"/>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>인간 공격</t>
-        </is>
-      </c>
+      <c r="A82" t="inlineStr"/>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>페이크 사기</t>
-        </is>
-      </c>
+      <c r="A83" t="inlineStr"/>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>지배</t>
-        </is>
-      </c>
+      <c r="A84" t="inlineStr"/>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>위험성 만점</t>
-        </is>
-      </c>
+      <c r="A85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>악용 우려</t>
-        </is>
-      </c>
+      <c r="A86" t="inlineStr"/>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>데이터 학습</t>
-        </is>
-      </c>
+      <c r="A87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>윤리 문제 발생</t>
-        </is>
-      </c>
+      <c r="A88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>해킹 위험</t>
-        </is>
-      </c>
+      <c r="A89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>도덕</t>
-        </is>
-      </c>
+      <c r="A90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>문학 의미</t>
-        </is>
-      </c>
+      <c r="A91" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>세상 지배</t>
-        </is>
-      </c>
+      <c r="A92" t="inlineStr"/>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>자연 파괴</t>
-        </is>
-      </c>
+      <c r="A93" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>범죄 악용</t>
-        </is>
-      </c>
+      <c r="A94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>사기 발생</t>
-        </is>
-      </c>
+      <c r="A95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>사람 범죄 악용</t>
-        </is>
-      </c>
+      <c r="A96" t="inlineStr"/>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>범죄</t>
-        </is>
-      </c>
+      <c r="A97" t="inlineStr"/>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>사이버 범죄</t>
-        </is>
-      </c>
+      <c r="A98" t="inlineStr"/>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>반란</t>
-        </is>
-      </c>
+      <c r="A99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>오류</t>
-        </is>
-      </c>
+      <c r="A100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>대한 규제</t>
-        </is>
-      </c>
+      <c r="A101" t="inlineStr"/>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>직업</t>
-        </is>
-      </c>
+      <c r="A102" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>